<commit_message>
add barcode mismatch param
</commit_message>
<xml_diff>
--- a/assets/extended_sample_sheet_template.xlsx
+++ b/assets/extended_sample_sheet_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonas/Documents/Projects/git/solo-in-drops/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC8D565-7A4C-BB4B-9BC6-79AA8D7BF930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FA810C-B3AD-014A-BC28-B9F985411B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16300" yWindow="3180" windowWidth="28040" windowHeight="19660" xr2:uid="{89D7250D-3031-744F-86EA-F02C8FEC9E50}"/>
+    <workbookView xWindow="16280" yWindow="3140" windowWidth="28040" windowHeight="19660" xr2:uid="{89D7250D-3031-744F-86EA-F02C8FEC9E50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="53">
   <si>
     <t>sample_id</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>tumor; patient_id</t>
+  </si>
+  <si>
+    <t>seq_run_id</t>
+  </si>
+  <si>
+    <t>210810_NB551189_0075_AHVMWGBGXJ</t>
   </si>
 </sst>
 </file>
@@ -544,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E5AF6B5-AAC6-EE4F-89CE-94FE488566FF}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,19 +561,20 @@
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -578,37 +585,40 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>42</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -619,37 +629,40 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>3000</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>80</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>43</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>19</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>49</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -660,37 +673,40 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>3000</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>76</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>43</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>19</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>50</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -701,37 +717,40 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>17</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>3000</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>60</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>43</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>18</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>19</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>50</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -742,37 +761,40 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>3000</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>55</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>43</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>18</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>19</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>49</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -783,37 +805,40 @@
         <v>33</v>
       </c>
       <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>17</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>3000</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>77</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>43</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>18</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>19</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>50</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -824,37 +849,40 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>3000</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>66</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>43</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>18</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>19</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>49</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -865,37 +893,40 @@
         <v>35</v>
       </c>
       <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>14</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>17</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>3000</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>90</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>43</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>18</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>19</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>50</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -906,37 +937,40 @@
         <v>36</v>
       </c>
       <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>14</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>17</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>3000</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>96</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>43</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>18</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>19</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>49</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -947,37 +981,40 @@
         <v>37</v>
       </c>
       <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
         <v>13</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>40</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>17</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>3000</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>45</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>43</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>18</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>41</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>50</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -988,37 +1025,40 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
         <v>13</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>40</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>17</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>3000</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>70</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>44</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>18</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>41</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>50</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1029,37 +1069,40 @@
         <v>39</v>
       </c>
       <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s">
         <v>13</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>40</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>17</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>3000</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>58</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>44</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>18</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>41</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>49</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1070,33 +1113,36 @@
         <v>48</v>
       </c>
       <c r="D13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
         <v>13</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>40</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>17</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>3000</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>88</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>44</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>18</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>41</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>50</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>